<commit_message>
pertemuan 14 - 13/07/2025
</commit_message>
<xml_diff>
--- a/uts/Rekap Nilai Ujian Tengah Semester Pelatihan React Java PUB 22.xlsx
+++ b/uts/Rekap Nilai Ujian Tengah Semester Pelatihan React Java PUB 22.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>No.</t>
   </si>
@@ -35,13 +35,55 @@
     <t>Nama</t>
   </si>
   <si>
-    <t>Nilai UTS</t>
-  </si>
-  <si>
-    <t>Angka</t>
-  </si>
-  <si>
-    <t>Grade</t>
+    <t>Entitas</t>
+  </si>
+  <si>
+    <t>Relasi</t>
+  </si>
+  <si>
+    <t>Anotasi JPA &amp; Lombok</t>
+  </si>
+  <si>
+    <t>Repository</t>
+  </si>
+  <si>
+    <t>Custom method search</t>
+  </si>
+  <si>
+    <t>Custom method sort</t>
+  </si>
+  <si>
+    <t>CRUD Lengkap</t>
+  </si>
+  <si>
+    <t>Endpoint search</t>
+  </si>
+  <si>
+    <t>Endpoint sorting</t>
+  </si>
+  <si>
+    <t>Jumlah controller</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Arjun Zebua</t>
+  </si>
+  <si>
+    <t>Dwi Wahyu S</t>
+  </si>
+  <si>
+    <t>Imelda Novianty</t>
+  </si>
+  <si>
+    <t>Mora Fidela</t>
+  </si>
+  <si>
+    <t>Patimah Sari</t>
+  </si>
+  <si>
+    <t>Sopiah Pasaribu</t>
   </si>
 </sst>
 </file>
@@ -54,7 +96,7 @@
     <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,13 +118,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -227,7 +262,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +271,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -421,12 +468,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -530,85 +592,79 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -617,10 +673,10 @@
     <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -629,10 +685,10 @@
     <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -641,10 +697,10 @@
     <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -653,10 +709,10 @@
     <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -665,29 +721,57 @@
     <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -749,13 +833,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
-<customStorage xmlns="https://web.wps.cn/et/2018/main">
-  <book/>
-  <sheets/>
-</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1016,22 +1093,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B4:E11"/>
+  <dimension ref="B4:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="9" style="2"/>
     <col min="3" max="3" width="20.7777777777778" style="1" customWidth="1"/>
     <col min="4" max="5" width="15.7777777777778" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
+    <col min="6" max="14" width="15.7777777777778" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:14">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1041,53 +1119,357 @@
       <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:14">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="11"/>
+    </row>
+    <row r="6" spans="2:14">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="6">
+        <v>20</v>
+      </c>
+      <c r="E6" s="6">
+        <v>5</v>
+      </c>
+      <c r="F6" s="7">
+        <v>5</v>
+      </c>
+      <c r="G6" s="7">
+        <v>5</v>
+      </c>
+      <c r="H6" s="7">
+        <v>5</v>
+      </c>
+      <c r="I6" s="7">
+        <v>5</v>
+      </c>
+      <c r="J6" s="7">
+        <v>20</v>
+      </c>
+      <c r="K6" s="7">
+        <v>5</v>
+      </c>
+      <c r="L6" s="7">
+        <v>5</v>
+      </c>
+      <c r="M6" s="7">
+        <v>5</v>
+      </c>
+      <c r="N6" s="12">
+        <f>SUM(D6:M6)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14">
+      <c r="B7" s="8">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="10">
+        <v>20</v>
+      </c>
+      <c r="E7" s="10">
+        <v>5</v>
+      </c>
+      <c r="F7" s="10">
+        <v>5</v>
+      </c>
+      <c r="G7" s="10">
+        <v>5</v>
+      </c>
+      <c r="H7" s="10">
+        <v>5</v>
+      </c>
+      <c r="I7" s="10">
+        <v>5</v>
+      </c>
+      <c r="J7" s="10">
+        <v>20</v>
+      </c>
+      <c r="K7" s="10">
+        <v>5</v>
+      </c>
+      <c r="L7" s="10">
+        <v>5</v>
+      </c>
+      <c r="M7" s="10">
+        <v>5</v>
+      </c>
+      <c r="N7" s="13">
+        <f>SUM(D7:M7)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14">
+      <c r="B8" s="8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="10">
+        <v>20</v>
+      </c>
+      <c r="E8" s="10">
+        <v>5</v>
+      </c>
+      <c r="F8" s="10">
+        <v>5</v>
+      </c>
+      <c r="G8" s="10">
+        <v>5</v>
+      </c>
+      <c r="H8" s="10">
+        <v>5</v>
+      </c>
+      <c r="I8" s="10">
+        <v>5</v>
+      </c>
+      <c r="J8" s="10">
+        <v>20</v>
+      </c>
+      <c r="K8" s="10">
+        <v>5</v>
+      </c>
+      <c r="L8" s="10">
+        <v>5</v>
+      </c>
+      <c r="M8" s="10">
+        <v>5</v>
+      </c>
+      <c r="N8" s="13">
+        <f>SUM(D8:M8)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14">
+      <c r="B9" s="8">
         <v>3</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="C9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="10">
+        <v>20</v>
+      </c>
+      <c r="E9" s="10">
+        <v>5</v>
+      </c>
+      <c r="F9" s="10">
+        <v>5</v>
+      </c>
+      <c r="G9" s="10">
+        <v>5</v>
+      </c>
+      <c r="H9" s="10">
+        <v>5</v>
+      </c>
+      <c r="I9" s="10">
+        <v>5</v>
+      </c>
+      <c r="J9" s="10">
+        <v>20</v>
+      </c>
+      <c r="K9" s="10">
+        <v>5</v>
+      </c>
+      <c r="L9" s="10">
+        <v>5</v>
+      </c>
+      <c r="M9" s="10">
+        <v>5</v>
+      </c>
+      <c r="N9" s="13">
+        <f>SUM(D9:M9)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14">
+      <c r="B10" s="8">
         <v>4</v>
       </c>
+      <c r="C10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="10">
+        <v>20</v>
+      </c>
+      <c r="E10" s="10">
+        <v>5</v>
+      </c>
+      <c r="F10" s="10">
+        <v>5</v>
+      </c>
+      <c r="G10" s="10">
+        <v>5</v>
+      </c>
+      <c r="H10" s="10">
+        <v>5</v>
+      </c>
+      <c r="I10" s="10">
+        <v>5</v>
+      </c>
+      <c r="J10" s="10">
+        <v>20</v>
+      </c>
+      <c r="K10" s="10">
+        <v>5</v>
+      </c>
+      <c r="L10" s="10">
+        <v>5</v>
+      </c>
+      <c r="M10" s="10">
+        <v>5</v>
+      </c>
+      <c r="N10" s="13">
+        <f>SUM(D10:M10)</f>
+        <v>80</v>
+      </c>
     </row>
-    <row r="6" spans="2:2">
-      <c r="B6" s="2">
-        <v>1</v>
+    <row r="11" spans="2:14">
+      <c r="B11" s="8">
+        <v>5</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="10">
+        <v>20</v>
+      </c>
+      <c r="E11" s="10">
+        <v>5</v>
+      </c>
+      <c r="F11" s="10">
+        <v>5</v>
+      </c>
+      <c r="G11" s="10">
+        <v>5</v>
+      </c>
+      <c r="H11" s="10">
+        <v>5</v>
+      </c>
+      <c r="I11" s="10">
+        <v>5</v>
+      </c>
+      <c r="J11" s="10">
+        <v>20</v>
+      </c>
+      <c r="K11" s="10">
+        <v>5</v>
+      </c>
+      <c r="L11" s="10">
+        <v>5</v>
+      </c>
+      <c r="M11" s="10">
+        <v>5</v>
+      </c>
+      <c r="N11" s="13">
+        <f>SUM(D11:M11)</f>
+        <v>80</v>
       </c>
     </row>
-    <row r="7" spans="2:2">
-      <c r="B7" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2">
-      <c r="B8" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2">
-      <c r="B9" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2">
-      <c r="B10" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2">
-      <c r="B11" s="2">
+    <row r="12" spans="2:14">
+      <c r="B12" s="8">
         <v>6</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="10">
+        <v>20</v>
+      </c>
+      <c r="E12" s="10">
+        <v>5</v>
+      </c>
+      <c r="F12" s="10">
+        <v>5</v>
+      </c>
+      <c r="G12" s="10">
+        <v>5</v>
+      </c>
+      <c r="H12" s="10">
+        <v>5</v>
+      </c>
+      <c r="I12" s="10">
+        <v>5</v>
+      </c>
+      <c r="J12" s="10">
+        <v>20</v>
+      </c>
+      <c r="K12" s="10">
+        <v>5</v>
+      </c>
+      <c r="L12" s="10">
+        <v>5</v>
+      </c>
+      <c r="M12" s="10">
+        <v>5</v>
+      </c>
+      <c r="N12" s="13">
+        <f>SUM(D12:M12)</f>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
+  <mergeCells count="13">
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>